<commit_message>
Updated results per country with overall demand
</commit_message>
<xml_diff>
--- a/Outputs/PtX_demand_AT.xlsx
+++ b/Outputs/PtX_demand_AT.xlsx
@@ -499,9 +499,15 @@
       <c r="B2" t="n">
         <v>2030</v>
       </c>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
+      <c r="C2" t="n">
+        <v>0.005275666120273866</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.008851734721773526</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.01430471668413269</v>
+      </c>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
@@ -723,9 +729,15 @@
       <c r="B12" t="n">
         <v>2040</v>
       </c>
-      <c r="C12" t="inlineStr"/>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
+      <c r="C12" t="n">
+        <v>0.02218391830577439</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.01011012915445557</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.02168455665835297</v>
+      </c>
       <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr"/>
@@ -951,9 +963,15 @@
       <c r="B22" t="n">
         <v>2050</v>
       </c>
-      <c r="C22" t="inlineStr"/>
-      <c r="D22" t="inlineStr"/>
-      <c r="E22" t="inlineStr"/>
+      <c r="C22" t="n">
+        <v>0.05806349380617117</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.01132223274949354</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.03488305184526833</v>
+      </c>
       <c r="F22" t="inlineStr"/>
       <c r="G22" t="inlineStr"/>
       <c r="H22" t="inlineStr"/>

</xml_diff>

<commit_message>
Updated Outputs folder with correct categories annd Aviation
</commit_message>
<xml_diff>
--- a/Outputs/PtX_demand_AT.xlsx
+++ b/Outputs/PtX_demand_AT.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K31"/>
+  <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -606,7 +606,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Synthetic Liquids</t>
+          <t>Fossil Gases</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -615,17 +615,21 @@
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
+      <c r="F7" t="n">
+        <v>0.001869582009059</v>
+      </c>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
+      <c r="I7" t="n">
+        <v>0.0001635093396769129</v>
+      </c>
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Biogenic Liquids</t>
+          <t>Synthetic Liquids</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -634,29 +638,17 @@
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr"/>
-      <c r="F8" t="n">
-        <v>0.0088988022673677</v>
-      </c>
-      <c r="G8" t="n">
-        <v>0.0002490546233072</v>
-      </c>
-      <c r="H8" t="n">
-        <v>1.935820348377023e-05</v>
-      </c>
-      <c r="I8" t="n">
-        <v>0.0075029523755567</v>
-      </c>
-      <c r="J8" t="n">
-        <v>0.0004216652327745</v>
-      </c>
-      <c r="K8" t="n">
-        <v>0.0001424131506473</v>
-      </c>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Biomass [Solid]</t>
+          <t>Biogenic Liquids</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -664,20 +656,30 @@
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr"/>
-      <c r="E9" t="n">
-        <v>0.01236568429895008</v>
-      </c>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="n">
+        <v>0.0088988022673677</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.0002490546233072</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.00294068626328137</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.0075029523755567</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0.0004216652327745</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.0001424131506473</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Renewable Energy Carrier</t>
+          <t>Fossil Liquids</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -685,174 +687,178 @@
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr"/>
-      <c r="E10" t="n">
-        <v>0.0004566597868233623</v>
-      </c>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="n">
+        <v>0.08829551818042421</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.0017540186779005</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.026856640122734</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.0487976340000506</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.0025523405410916</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.001018155413845</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Overall Demand</t>
+          <t>Biomass [Solid]</t>
         </is>
       </c>
       <c r="B11" t="n">
         <v>2030</v>
       </c>
-      <c r="C11" t="n">
-        <v>0.005275666120273866</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0.008851734721773525</v>
-      </c>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr"/>
       <c r="E11" t="n">
-        <v>0.0143047166841327</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0.009531225782117271</v>
-      </c>
-      <c r="G11" t="n">
-        <v>0.0002490546233072</v>
-      </c>
-      <c r="H11" t="n">
-        <v>1.935931871364941e-05</v>
-      </c>
-      <c r="I11" t="n">
-        <v>0.007736027499871657</v>
-      </c>
-      <c r="J11" t="n">
-        <v>0.0004216652327745</v>
-      </c>
-      <c r="K11" t="n">
-        <v>0.0001424131506473</v>
-      </c>
+        <v>0.01236568429895008</v>
+      </c>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Hydrogen</t>
+          <t>Renewable Energy Carrier</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>2040</v>
-      </c>
-      <c r="C12" t="n">
-        <v>0.02218391830577439</v>
-      </c>
+        <v>2030</v>
+      </c>
+      <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="n">
-        <v>0.0023340995429285</v>
-      </c>
+      <c r="E12" t="n">
+        <v>0.0004566597868233623</v>
+      </c>
+      <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr"/>
-      <c r="H12" t="n">
-        <v>9.335705868852003e-08</v>
-      </c>
-      <c r="I12" t="n">
-        <v>0.0002938140845309541</v>
-      </c>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Methanol</t>
+          <t>Overall Demand</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>2040</v>
-      </c>
-      <c r="C13" t="inlineStr"/>
+        <v>2030</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.005275666120273866</v>
+      </c>
       <c r="D13" t="n">
-        <v>0.0001395199360307602</v>
-      </c>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr"/>
-      <c r="K13" t="inlineStr"/>
+        <v>0.008851734721773525</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.0143047166841327</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.09969632597160048</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.0020030733012077</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.02979732750124525</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.05669717083959917</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0.0029740057738661</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0.0011605685644923</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Ammonia</t>
+          <t>Hydrogen</t>
         </is>
       </c>
       <c r="B14" t="n">
         <v>2040</v>
       </c>
-      <c r="C14" t="inlineStr"/>
-      <c r="D14" t="n">
-        <v>0.009970609218424816</v>
-      </c>
+      <c r="C14" t="n">
+        <v>0.02218391830577439</v>
+      </c>
+      <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr"/>
-      <c r="F14" t="inlineStr"/>
+      <c r="F14" t="n">
+        <v>0.0023340995429285</v>
+      </c>
       <c r="G14" t="inlineStr"/>
-      <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr"/>
+      <c r="H14" t="n">
+        <v>9.335705868852003e-08</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.0002938140845309541</v>
+      </c>
       <c r="J14" t="inlineStr"/>
       <c r="K14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Synthetic Gases</t>
+          <t>Methanol</t>
         </is>
       </c>
       <c r="B15" t="n">
         <v>2040</v>
       </c>
       <c r="C15" t="inlineStr"/>
-      <c r="D15" t="inlineStr"/>
+      <c r="D15" t="n">
+        <v>0.0001395199360307602</v>
+      </c>
       <c r="E15" t="inlineStr"/>
-      <c r="F15" t="n">
-        <v>8.529267033332886e-10</v>
-      </c>
+      <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr"/>
       <c r="H15" t="inlineStr"/>
-      <c r="I15" t="n">
-        <v>1.030000188038228e-10</v>
-      </c>
+      <c r="I15" t="inlineStr"/>
       <c r="J15" t="inlineStr"/>
       <c r="K15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Biogenic Gases</t>
+          <t>Ammonia</t>
         </is>
       </c>
       <c r="B16" t="n">
         <v>2040</v>
       </c>
       <c r="C16" t="inlineStr"/>
-      <c r="D16" t="inlineStr"/>
-      <c r="E16" t="n">
-        <v>0.006236696536118492</v>
-      </c>
-      <c r="F16" t="n">
-        <v>0.0001811189577034403</v>
-      </c>
+      <c r="D16" t="n">
+        <v>0.009970609218424816</v>
+      </c>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr"/>
       <c r="G16" t="inlineStr"/>
       <c r="H16" t="inlineStr"/>
-      <c r="I16" t="n">
-        <v>7.116808198921916e-05</v>
-      </c>
+      <c r="I16" t="inlineStr"/>
       <c r="J16" t="inlineStr"/>
       <c r="K16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Synthetic Liquids</t>
+          <t>Synthetic Gases</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -861,17 +867,21 @@
       <c r="C17" t="inlineStr"/>
       <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr"/>
-      <c r="F17" t="inlineStr"/>
+      <c r="F17" t="n">
+        <v>8.529267033332886e-10</v>
+      </c>
       <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr"/>
-      <c r="I17" t="inlineStr"/>
+      <c r="I17" t="n">
+        <v>1.030000188038228e-10</v>
+      </c>
       <c r="J17" t="inlineStr"/>
       <c r="K17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Biogenic Liquids</t>
+          <t>Biogenic Gases</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -879,30 +889,24 @@
       </c>
       <c r="C18" t="inlineStr"/>
       <c r="D18" t="inlineStr"/>
-      <c r="E18" t="inlineStr"/>
+      <c r="E18" t="n">
+        <v>0.006236696536118492</v>
+      </c>
       <c r="F18" t="n">
-        <v>0.003933003359716599</v>
-      </c>
-      <c r="G18" t="n">
-        <v>0.0004060001237347</v>
-      </c>
-      <c r="H18" t="n">
-        <v>3.005616220791097e-05</v>
-      </c>
+        <v>0.0001811189577034403</v>
+      </c>
+      <c r="G18" t="inlineStr"/>
+      <c r="H18" t="inlineStr"/>
       <c r="I18" t="n">
-        <v>0.0051493834043723</v>
-      </c>
-      <c r="J18" t="n">
-        <v>0.000512254822244</v>
-      </c>
-      <c r="K18" t="n">
-        <v>0.0001870184333603</v>
-      </c>
+        <v>7.116808198921916e-05</v>
+      </c>
+      <c r="J18" t="inlineStr"/>
+      <c r="K18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Biomass [Solid]</t>
+          <t>Fossil Gases</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -910,20 +914,22 @@
       </c>
       <c r="C19" t="inlineStr"/>
       <c r="D19" t="inlineStr"/>
-      <c r="E19" t="n">
-        <v>0.01390636056580271</v>
-      </c>
-      <c r="F19" t="inlineStr"/>
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="n">
+        <v>0.0010115703017416</v>
+      </c>
       <c r="G19" t="inlineStr"/>
       <c r="H19" t="inlineStr"/>
-      <c r="I19" t="inlineStr"/>
+      <c r="I19" t="n">
+        <v>0.0001773145296588229</v>
+      </c>
       <c r="J19" t="inlineStr"/>
       <c r="K19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Renewable Energy Carrier</t>
+          <t>Synthetic Liquids</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -931,9 +937,7 @@
       </c>
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr"/>
-      <c r="E20" t="n">
-        <v>0.001541499556431764</v>
-      </c>
+      <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr"/>
@@ -944,32 +948,26 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Overall Demand</t>
+          <t>Biogenic Liquids</t>
         </is>
       </c>
       <c r="B21" t="n">
         <v>2040</v>
       </c>
-      <c r="C21" t="n">
-        <v>0.02218391830577439</v>
-      </c>
-      <c r="D21" t="n">
-        <v>0.01011012915445558</v>
-      </c>
-      <c r="E21" t="n">
-        <v>0.02168455665835297</v>
-      </c>
+      <c r="C21" t="inlineStr"/>
+      <c r="D21" t="inlineStr"/>
+      <c r="E21" t="inlineStr"/>
       <c r="F21" t="n">
-        <v>0.006448222713275243</v>
+        <v>0.003933003359716599</v>
       </c>
       <c r="G21" t="n">
         <v>0.0004060001237347</v>
       </c>
       <c r="H21" t="n">
-        <v>3.014951926659949e-05</v>
+        <v>0.003586355591096711</v>
       </c>
       <c r="I21" t="n">
-        <v>0.005514365673892492</v>
+        <v>0.0051493834043723</v>
       </c>
       <c r="J21" t="n">
         <v>0.000512254822244</v>
@@ -981,44 +979,48 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Hydrogen</t>
+          <t>Fossil Liquids</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>2050</v>
-      </c>
-      <c r="C22" t="n">
-        <v>0.05806349380617117</v>
-      </c>
+        <v>2040</v>
+      </c>
+      <c r="C22" t="inlineStr"/>
       <c r="D22" t="inlineStr"/>
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="n">
-        <v>0.0032371523854854</v>
-      </c>
-      <c r="G22" t="inlineStr"/>
+        <v>0.0248606019595066</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0.0018856675971865</v>
+      </c>
       <c r="H22" t="n">
-        <v>1.582326947158595e-07</v>
+        <v>0.0253236759528751</v>
       </c>
       <c r="I22" t="n">
-        <v>0.0004748991182328069</v>
-      </c>
-      <c r="J22" t="inlineStr"/>
-      <c r="K22" t="inlineStr"/>
+        <v>0.0227039295093894</v>
+      </c>
+      <c r="J22" t="n">
+        <v>0.0022649738849363</v>
+      </c>
+      <c r="K22" t="n">
+        <v>0.0008983383025388</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Methanol</t>
+          <t>Biomass [Solid]</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>2050</v>
+        <v>2040</v>
       </c>
       <c r="C23" t="inlineStr"/>
-      <c r="D23" t="n">
-        <v>0.0001562469840692931</v>
-      </c>
-      <c r="E23" t="inlineStr"/>
+      <c r="D23" t="inlineStr"/>
+      <c r="E23" t="n">
+        <v>0.01390636056580271</v>
+      </c>
       <c r="F23" t="inlineStr"/>
       <c r="G23" t="inlineStr"/>
       <c r="H23" t="inlineStr"/>
@@ -1029,17 +1031,17 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Ammonia</t>
+          <t>Renewable Energy Carrier</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>2050</v>
+        <v>2040</v>
       </c>
       <c r="C24" t="inlineStr"/>
-      <c r="D24" t="n">
-        <v>0.01116598576542424</v>
-      </c>
-      <c r="E24" t="inlineStr"/>
+      <c r="D24" t="inlineStr"/>
+      <c r="E24" t="n">
+        <v>0.001541499556431764</v>
+      </c>
       <c r="F24" t="inlineStr"/>
       <c r="G24" t="inlineStr"/>
       <c r="H24" t="inlineStr"/>
@@ -1050,47 +1052,63 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Synthetic Gases</t>
+          <t>Overall Demand</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>2050</v>
-      </c>
-      <c r="C25" t="inlineStr"/>
-      <c r="D25" t="inlineStr"/>
-      <c r="E25" t="inlineStr"/>
+        <v>2040</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0.02218391830577439</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0.01011012915445558</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0.02168455665835297</v>
+      </c>
       <c r="F25" t="n">
-        <v>7.829013935122213e-09</v>
-      </c>
-      <c r="G25" t="inlineStr"/>
-      <c r="H25" t="inlineStr"/>
+        <v>0.03232039497452344</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0.0022916677209212</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0.0289101249010305</v>
+      </c>
       <c r="I25" t="n">
-        <v>3.585644379015236e-09</v>
-      </c>
-      <c r="J25" t="inlineStr"/>
-      <c r="K25" t="inlineStr"/>
+        <v>0.02839560971294071</v>
+      </c>
+      <c r="J25" t="n">
+        <v>0.0027772287071803</v>
+      </c>
+      <c r="K25" t="n">
+        <v>0.0010853567358991</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Biogenic Gases</t>
+          <t>Hydrogen</t>
         </is>
       </c>
       <c r="B26" t="n">
         <v>2050</v>
       </c>
-      <c r="C26" t="inlineStr"/>
+      <c r="C26" t="n">
+        <v>0.05806349380617117</v>
+      </c>
       <c r="D26" t="inlineStr"/>
-      <c r="E26" t="n">
-        <v>0.01634275778491433</v>
-      </c>
+      <c r="E26" t="inlineStr"/>
       <c r="F26" t="n">
-        <v>3.081962227811797e-05</v>
+        <v>0.0032371523854854</v>
       </c>
       <c r="G26" t="inlineStr"/>
-      <c r="H26" t="inlineStr"/>
+      <c r="H26" t="n">
+        <v>1.582326947158595e-07</v>
+      </c>
       <c r="I26" t="n">
-        <v>1.931652100554092e-05</v>
+        <v>0.0004748991182328069</v>
       </c>
       <c r="J26" t="inlineStr"/>
       <c r="K26" t="inlineStr"/>
@@ -1098,69 +1116,49 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Synthetic Liquids</t>
+          <t>Methanol</t>
         </is>
       </c>
       <c r="B27" t="n">
         <v>2050</v>
       </c>
       <c r="C27" t="inlineStr"/>
-      <c r="D27" t="inlineStr"/>
+      <c r="D27" t="n">
+        <v>0.0001562469840692931</v>
+      </c>
       <c r="E27" t="inlineStr"/>
-      <c r="F27" t="n">
-        <v>3.727194664208952e-11</v>
-      </c>
-      <c r="G27" t="n">
-        <v>1.495079014282506e-11</v>
-      </c>
-      <c r="H27" t="n">
-        <v>6.271052964305957e-13</v>
-      </c>
-      <c r="I27" t="n">
-        <v>7.863278190362155e-11</v>
-      </c>
-      <c r="J27" t="n">
-        <v>3.50834399409891e-12</v>
-      </c>
-      <c r="K27" t="n">
-        <v>3.150512143598475e-11</v>
-      </c>
+      <c r="F27" t="inlineStr"/>
+      <c r="G27" t="inlineStr"/>
+      <c r="H27" t="inlineStr"/>
+      <c r="I27" t="inlineStr"/>
+      <c r="J27" t="inlineStr"/>
+      <c r="K27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Biogenic Liquids</t>
+          <t>Ammonia</t>
         </is>
       </c>
       <c r="B28" t="n">
         <v>2050</v>
       </c>
       <c r="C28" t="inlineStr"/>
-      <c r="D28" t="inlineStr"/>
+      <c r="D28" t="n">
+        <v>0.01116598576542424</v>
+      </c>
       <c r="E28" t="inlineStr"/>
-      <c r="F28" t="n">
-        <v>0.0005043429529444853</v>
-      </c>
-      <c r="G28" t="n">
-        <v>0.0007254509390932</v>
-      </c>
-      <c r="H28" t="n">
-        <v>4.748745208470587e-05</v>
-      </c>
-      <c r="I28" t="n">
-        <v>0.001343316704467</v>
-      </c>
-      <c r="J28" t="n">
-        <v>0.0006588408195702</v>
-      </c>
-      <c r="K28" t="n">
-        <v>0.0002539892107095</v>
-      </c>
+      <c r="F28" t="inlineStr"/>
+      <c r="G28" t="inlineStr"/>
+      <c r="H28" t="inlineStr"/>
+      <c r="I28" t="inlineStr"/>
+      <c r="J28" t="inlineStr"/>
+      <c r="K28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Biomass [Solid]</t>
+          <t>Synthetic Gases</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -1168,20 +1166,22 @@
       </c>
       <c r="C29" t="inlineStr"/>
       <c r="D29" t="inlineStr"/>
-      <c r="E29" t="n">
-        <v>0.01548483145203032</v>
-      </c>
-      <c r="F29" t="inlineStr"/>
+      <c r="E29" t="inlineStr"/>
+      <c r="F29" t="n">
+        <v>7.829013935122213e-09</v>
+      </c>
       <c r="G29" t="inlineStr"/>
       <c r="H29" t="inlineStr"/>
-      <c r="I29" t="inlineStr"/>
+      <c r="I29" t="n">
+        <v>3.585644379015236e-09</v>
+      </c>
       <c r="J29" t="inlineStr"/>
       <c r="K29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Renewable Energy Carrier</t>
+          <t>Biogenic Gases</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -1190,50 +1190,212 @@
       <c r="C30" t="inlineStr"/>
       <c r="D30" t="inlineStr"/>
       <c r="E30" t="n">
-        <v>0.003055462608323681</v>
-      </c>
-      <c r="F30" t="inlineStr"/>
+        <v>0.01634275778491433</v>
+      </c>
+      <c r="F30" t="n">
+        <v>3.081962227811797e-05</v>
+      </c>
       <c r="G30" t="inlineStr"/>
       <c r="H30" t="inlineStr"/>
-      <c r="I30" t="inlineStr"/>
+      <c r="I30" t="n">
+        <v>1.931652100554092e-05</v>
+      </c>
       <c r="J30" t="inlineStr"/>
       <c r="K30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Overall Demand</t>
+          <t>Fossil Gases</t>
         </is>
       </c>
       <c r="B31" t="n">
         <v>2050</v>
       </c>
-      <c r="C31" t="n">
+      <c r="C31" t="inlineStr"/>
+      <c r="D31" t="inlineStr"/>
+      <c r="E31" t="inlineStr"/>
+      <c r="F31" t="n">
+        <v>6.233856403552209e-05</v>
+      </c>
+      <c r="G31" t="inlineStr"/>
+      <c r="H31" t="inlineStr"/>
+      <c r="I31" t="n">
+        <v>6.033626251213144e-05</v>
+      </c>
+      <c r="J31" t="inlineStr"/>
+      <c r="K31" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Synthetic Liquids</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>2050</v>
+      </c>
+      <c r="C32" t="inlineStr"/>
+      <c r="D32" t="inlineStr"/>
+      <c r="E32" t="inlineStr"/>
+      <c r="F32" t="n">
+        <v>3.727194664208952e-11</v>
+      </c>
+      <c r="G32" t="n">
+        <v>1.495079014282506e-11</v>
+      </c>
+      <c r="H32" t="n">
+        <v>1.376416589452187e-10</v>
+      </c>
+      <c r="I32" t="n">
+        <v>7.863278190362155e-11</v>
+      </c>
+      <c r="J32" t="n">
+        <v>3.50834399409891e-12</v>
+      </c>
+      <c r="K32" t="n">
+        <v>3.150512143598475e-11</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Biogenic Liquids</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>2050</v>
+      </c>
+      <c r="C33" t="inlineStr"/>
+      <c r="D33" t="inlineStr"/>
+      <c r="E33" t="inlineStr"/>
+      <c r="F33" t="n">
+        <v>0.0005043429529444853</v>
+      </c>
+      <c r="G33" t="n">
+        <v>0.0007254509390932</v>
+      </c>
+      <c r="H33" t="n">
+        <v>0.004705473489427407</v>
+      </c>
+      <c r="I33" t="n">
+        <v>0.001343316704467</v>
+      </c>
+      <c r="J33" t="n">
+        <v>0.0006588408195702</v>
+      </c>
+      <c r="K33" t="n">
+        <v>0.0002539892107095</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Fossil Liquids</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>2050</v>
+      </c>
+      <c r="C34" t="inlineStr"/>
+      <c r="D34" t="inlineStr"/>
+      <c r="E34" t="inlineStr"/>
+      <c r="F34" t="n">
+        <v>0.0022828303593454</v>
+      </c>
+      <c r="G34" t="n">
+        <v>0.0017007923139726</v>
+      </c>
+      <c r="H34" t="n">
+        <v>0.022936967601032</v>
+      </c>
+      <c r="I34" t="n">
+        <v>0.003944120735888</v>
+      </c>
+      <c r="J34" t="n">
+        <v>0.0019495783044021</v>
+      </c>
+      <c r="K34" t="n">
+        <v>0.0007373195447192</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Biomass [Solid]</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>2050</v>
+      </c>
+      <c r="C35" t="inlineStr"/>
+      <c r="D35" t="inlineStr"/>
+      <c r="E35" t="n">
+        <v>0.01548483145203032</v>
+      </c>
+      <c r="F35" t="inlineStr"/>
+      <c r="G35" t="inlineStr"/>
+      <c r="H35" t="inlineStr"/>
+      <c r="I35" t="inlineStr"/>
+      <c r="J35" t="inlineStr"/>
+      <c r="K35" t="inlineStr"/>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Renewable Energy Carrier</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>2050</v>
+      </c>
+      <c r="C36" t="inlineStr"/>
+      <c r="D36" t="inlineStr"/>
+      <c r="E36" t="n">
+        <v>0.003055462608323681</v>
+      </c>
+      <c r="F36" t="inlineStr"/>
+      <c r="G36" t="inlineStr"/>
+      <c r="H36" t="inlineStr"/>
+      <c r="I36" t="inlineStr"/>
+      <c r="J36" t="inlineStr"/>
+      <c r="K36" t="inlineStr"/>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Overall Demand</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>2050</v>
+      </c>
+      <c r="C37" t="n">
         <v>0.05806349380617117</v>
       </c>
-      <c r="D31" t="n">
+      <c r="D37" t="n">
         <v>0.01132223274949354</v>
       </c>
-      <c r="E31" t="n">
+      <c r="E37" t="n">
         <v>0.03488305184526833</v>
       </c>
-      <c r="F31" t="n">
-        <v>0.003772322826993885</v>
-      </c>
-      <c r="G31" t="n">
-        <v>0.0007254509540439902</v>
-      </c>
-      <c r="H31" t="n">
-        <v>4.764568540652703e-05</v>
-      </c>
-      <c r="I31" t="n">
-        <v>0.001837536007982509</v>
-      </c>
-      <c r="J31" t="n">
-        <v>0.000658840823078544</v>
-      </c>
-      <c r="K31" t="n">
-        <v>0.0002539892422146214</v>
+      <c r="F37" t="n">
+        <v>0.006117491750374807</v>
+      </c>
+      <c r="G37" t="n">
+        <v>0.00242624326801659</v>
+      </c>
+      <c r="H37" t="n">
+        <v>0.02764259946079578</v>
+      </c>
+      <c r="I37" t="n">
+        <v>0.00584199300638264</v>
+      </c>
+      <c r="J37" t="n">
+        <v>0.002608419127480644</v>
+      </c>
+      <c r="K37" t="n">
+        <v>0.0009913087869338215</v>
       </c>
     </row>
   </sheetData>

</xml_diff>